<commit_message>
revise according to review
</commit_message>
<xml_diff>
--- a/3/zssessentials/src/main/webapp/WEB-INF/books/protection.xlsx
+++ b/3/zssessentials/src/main/webapp/WEB-INF/books/protection.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>B2 is the only unlocked cell</t>
+    <t>B2 is unlocked</t>
   </si>
 </sst>
 </file>
@@ -439,12 +439,12 @@
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">

</xml_diff>